<commit_message>
errors evaluation fixed + new dataset added
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_4.1.xlsx
+++ b/input/calorimetry/test_4.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="targets" sheetId="6" r:id="rId6"/>
     <sheet name="enthalpies" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -1433,7 +1433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
@@ -2468,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2490,7 +2490,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-55810</v>
+        <v>55810</v>
       </c>
     </row>
   </sheetData>

</xml_diff>